<commit_message>
bao cao tien do
</commit_message>
<xml_diff>
--- a/BaoCaoTienDo.xlsx
+++ b/BaoCaoTienDo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Website-Ban-Sach\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>TIỂU LUẬN CHUYÊN NGÀNH</t>
   </si>
@@ -47,7 +47,19 @@
     <t>Kết quả thực hiện</t>
   </si>
   <si>
-    <t xml:space="preserve">Khảo sát </t>
+    <t>Khảo sát hiện trạng</t>
+  </si>
+  <si>
+    <t>hoàn thành</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vẽ use case </t>
+  </si>
+  <si>
+    <t>Tạo link github</t>
+  </si>
+  <si>
+    <t>Phát thảo công nghệ</t>
   </si>
 </sst>
 </file>
@@ -147,10 +159,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -435,7 +447,7 @@
   <dimension ref="B1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,13 +491,15 @@
       <c r="C4" s="3">
         <v>16110105</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
@@ -494,51 +508,63 @@
       <c r="C5" s="3">
         <v>16110206</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E8" s="9"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E9" s="9">
+      <c r="E9" s="10">
         <v>2</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="E14" s="6"/>

</xml_diff>